<commit_message>
update table format, font etc.
</commit_message>
<xml_diff>
--- a/outputs/torch/lstm.xlsx
+++ b/outputs/torch/lstm.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="details" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Details" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,13 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -43,7 +50,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -58,17 +65,63 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -457,196 +510,266 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>layer_l0</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>layer_l1</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>I1</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>I2</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>I3</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>O1</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>O2</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>O3</t>
-        </is>
-      </c>
-      <c r="I1" s="3" t="inlineStr">
-        <is>
-          <t>SizeI</t>
-        </is>
-      </c>
-      <c r="J1" s="3" t="inlineStr">
-        <is>
-          <t>SizeO</t>
-        </is>
-      </c>
-      <c r="K1" s="3" t="inlineStr">
-        <is>
-          <t>SizeW</t>
-        </is>
-      </c>
-      <c r="L1" s="3" t="inlineStr">
-        <is>
-          <t>OpGemm</t>
-        </is>
-      </c>
-      <c r="M1" s="3" t="inlineStr">
-        <is>
-          <t>OpElem</t>
-        </is>
-      </c>
-      <c r="N1" s="3" t="inlineStr">
-        <is>
-          <t>OpActi</t>
-        </is>
-      </c>
+      <c r="A1" s="10" t="inlineStr"/>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Layer Hierarchy</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="n"/>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>Input Dimension</t>
+        </is>
+      </c>
+      <c r="E1" s="12" t="n"/>
+      <c r="F1" s="11" t="n"/>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Output Dimension</t>
+        </is>
+      </c>
+      <c r="H1" s="12" t="n"/>
+      <c r="I1" s="11" t="n"/>
+      <c r="J1" s="10" t="inlineStr">
+        <is>
+          <t>Size of Parameters</t>
+        </is>
+      </c>
+      <c r="K1" s="12" t="n"/>
+      <c r="L1" s="11" t="n"/>
+      <c r="M1" s="10" t="inlineStr">
+        <is>
+          <t>Operation Summary</t>
+        </is>
+      </c>
+      <c r="N1" s="12" t="n"/>
+      <c r="O1" s="11" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Embedding: 1-1</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>300</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>300</v>
-      </c>
-      <c r="K2" t="n">
-        <v>9600</v>
-      </c>
-      <c r="L2" t="n">
-        <v>9600</v>
+      <c r="A2" s="13" t="inlineStr"/>
+      <c r="B2" s="13" t="inlineStr">
+        <is>
+          <t>L0</t>
+        </is>
+      </c>
+      <c r="C2" s="13" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="D2" s="13" t="inlineStr">
+        <is>
+          <t>I1</t>
+        </is>
+      </c>
+      <c r="E2" s="13" t="inlineStr">
+        <is>
+          <t>I2</t>
+        </is>
+      </c>
+      <c r="F2" s="13" t="inlineStr">
+        <is>
+          <t>I3</t>
+        </is>
+      </c>
+      <c r="G2" s="13" t="inlineStr">
+        <is>
+          <t>O1</t>
+        </is>
+      </c>
+      <c r="H2" s="13" t="inlineStr">
+        <is>
+          <t>O2</t>
+        </is>
+      </c>
+      <c r="I2" s="13" t="inlineStr">
+        <is>
+          <t>O3</t>
+        </is>
+      </c>
+      <c r="J2" s="13" t="inlineStr">
+        <is>
+          <t>Input</t>
+        </is>
+      </c>
+      <c r="K2" s="13" t="inlineStr">
+        <is>
+          <t>Output</t>
+        </is>
+      </c>
+      <c r="L2" s="13" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="M2" s="13" t="inlineStr">
+        <is>
+          <t>GEMM</t>
+        </is>
+      </c>
+      <c r="N2" s="13" t="inlineStr">
+        <is>
+          <t>ElemWise</t>
+        </is>
+      </c>
+      <c r="O2" s="13" t="inlineStr">
+        <is>
+          <t>Activation</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LSTM: 1-2</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="A3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>Embedding: 1-1</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="n"/>
+      <c r="D3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" s="8" t="n"/>
+      <c r="F3" s="8" t="n"/>
+      <c r="G3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="n">
         <v>300</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" s="8" t="n"/>
+      <c r="J3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="n">
-        <v>512</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="K3" s="8" t="n">
         <v>300</v>
       </c>
-      <c r="J3" t="n">
-        <v>512</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3768320</v>
-      </c>
-      <c r="L3" t="n">
-        <v>3768320</v>
-      </c>
-      <c r="N3" t="n">
-        <v>5120</v>
-      </c>
+      <c r="L3" s="8" t="n">
+        <v>9600</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <v>9600</v>
+      </c>
+      <c r="N3" s="8" t="n"/>
+      <c r="O3" s="8" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>LSTM: 1-2</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="n"/>
+      <c r="D4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="F4" s="8" t="n"/>
+      <c r="G4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>512</v>
+      </c>
+      <c r="I4" s="8" t="n"/>
+      <c r="J4" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="K4" s="8" t="n">
+        <v>512</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>3768320</v>
+      </c>
+      <c r="M4" s="8" t="n">
+        <v>3760128</v>
+      </c>
+      <c r="N4" s="8" t="n"/>
+      <c r="O4" s="8" t="n">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>Linear: 1-3</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" s="8" t="n"/>
+      <c r="D5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E5" s="8" t="n">
         <v>512</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" s="8" t="n"/>
+      <c r="G5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H5" s="8" t="n">
         <v>32</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I5" s="8" t="n"/>
+      <c r="J5" s="8" t="n">
         <v>512</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K5" s="8" t="n">
         <v>32</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L5" s="8" t="n">
         <v>16416</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M5" s="8" t="n">
         <v>16384</v>
       </c>
+      <c r="N5" s="8" t="n"/>
+      <c r="O5" s="8" t="n"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J1:J4">
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="K1:K5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>512</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K4">
+  <conditionalFormatting sqref="L1:L5">
     <cfRule type="cellIs" priority="2" operator="equal" dxfId="1" stopIfTrue="1">
       <formula>3768320</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L4">
+  <conditionalFormatting sqref="M1:M5">
     <cfRule type="cellIs" priority="3" operator="equal" dxfId="2" stopIfTrue="1">
-      <formula>3768320</formula>
+      <formula>3760128</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -671,40 +794,41 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>Model Statistics:</t>
         </is>
       </c>
+      <c r="B1" s="9" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Total Activations(MB):</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="8" t="n">
         <v>0.000844</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>Total Weights(MB):</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="8" t="n">
         <v>3.794336</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Total Gemm (G_ops):</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.003794304</v>
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>Total GEMM (G_ops):</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>0.003786112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>